<commit_message>
add comments for code
</commit_message>
<xml_diff>
--- a/spring-security-oauth2/doc/Client_Code_Review.xlsx
+++ b/spring-security-oauth2/doc/Client_Code_Review.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14640" windowHeight="7950" firstSheet="6" activeTab="7"/>
+    <workbookView windowWidth="15255" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_Class" sheetId="3" r:id="rId1"/>
@@ -168,7 +168,7 @@
   <si>
     <t>从上下文环境获取 accessToken Request
 从上下文获取access token
-如果为获取到，则使用accessTokenProvider 通过 oauth2 流程获取 accessToken</t>
+如果未获取到，则使用accessTokenProvider 通过 oauth2 流程获取 accessToken</t>
   </si>
   <si>
     <t>appendQueryParameter</t>
@@ -449,8 +449,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
@@ -524,32 +524,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -561,16 +546,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -585,15 +563,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -606,24 +591,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -644,15 +642,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -679,7 +679,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -691,7 +751,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -703,55 +811,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -763,19 +829,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -787,73 +853,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -920,41 +920,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -969,17 +934,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1002,8 +961,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1011,8 +985,34 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1024,10 +1024,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1036,16 +1036,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1054,115 +1054,115 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1666,7 +1666,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7118350"/>
-          <a:ext cx="8066405" cy="1733550"/>
+          <a:ext cx="8618855" cy="1733550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1708,7 +1708,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="10204450"/>
-          <a:ext cx="8752205" cy="4352290"/>
+          <a:ext cx="9304655" cy="4352290"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1750,7 +1750,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="635" y="15728950"/>
-          <a:ext cx="8733155" cy="4399915"/>
+          <a:ext cx="9285605" cy="4399915"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1792,7 +1792,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="635" y="25720675"/>
-          <a:ext cx="8504555" cy="4523740"/>
+          <a:ext cx="9057005" cy="4523740"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1834,7 +1834,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="635" y="20605750"/>
-          <a:ext cx="8752205" cy="4228465"/>
+          <a:ext cx="9304655" cy="4228465"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2204,8 +2204,8 @@
   <sheetPr/>
   <dimension ref="A1:W135"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="K90" sqref="K90"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="L118" sqref="L118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5"/>
@@ -2942,7 +2942,7 @@
   <sheetPr/>
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:W28"/>
     </sheetView>
   </sheetViews>
@@ -3392,7 +3392,7 @@
   <sheetPr/>
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView topLeftCell="E16" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A20" sqref="A20:W28"/>
     </sheetView>
   </sheetViews>
@@ -3671,7 +3671,7 @@
   <sheetPr/>
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F15" sqref="F15:I15"/>
     </sheetView>
   </sheetViews>
@@ -4273,13 +4273,15 @@
   <sheetPr/>
   <dimension ref="A1:W144"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A139" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="16384" width="5.625" customWidth="1"/>
+    <col min="1" max="4" width="5.625" customWidth="1"/>
+    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="6" max="16384" width="5.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" spans="1:1">
@@ -4957,7 +4959,7 @@
   <sheetPr/>
   <dimension ref="A2:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4985,7 +4987,7 @@
   <sheetPr/>
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>